<commit_message>
Fix Lat/Lon units in Power_VRES (-> v0.0.3r)
</commit_message>
<xml_diff>
--- a/examples/Power_VRES.xlsx
+++ b/examples/Power_VRES.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Frauental\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A4BA47-1C5A-4279-AEEA-10ED4845871D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C759EA27-F488-4721-B191-54D4E9491B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scenario" sheetId="107" r:id="rId1"/>
+    <sheet name="ScenarioA" sheetId="107" r:id="rId1"/>
+    <sheet name="ScenarioB" sheetId="108" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario!$C$3:$O$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScenarioA!$C$3:$O$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ScenarioB!$C$3:$O$11</definedName>
     <definedName name="businfo">#REF!</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
@@ -34,7 +36,8 @@
     <definedName name="inflows">#REF!</definedName>
     <definedName name="network">#REF!</definedName>
     <definedName name="param">#REF!</definedName>
-    <definedName name="renewable">scenario!$C$2:$O$644</definedName>
+    <definedName name="renewable" localSheetId="1">ScenarioB!$C$2:$O$644</definedName>
+    <definedName name="renewable">ScenarioA!$C$2:$O$644</definedName>
     <definedName name="resprofile">#REF!</definedName>
     <definedName name="runofriver">#REF!</definedName>
     <definedName name="sCodeName">#REF!</definedName>
@@ -156,8 +159,102 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Felix Auer</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{C2E04980-2AFA-4AC1-A87E-E4475FAC15F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If a line has a value in this column, it is not read in (i.e., does not exist).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{E6636B37-8F06-44DA-906F-2CF904D6935F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Readable Name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{7A314526-70B2-493B-B1B9-79942BC00B49}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value specifier in DB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{CC6DC82F-409F-4432-AE75-E7B07CADBD9D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Description</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{6768D181-C202-403A-A65D-F33E880F64F8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Details on database behavior</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{9A58A11F-9158-49F9-BCA3-2F9FB5F251E5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit or valid values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
   <si>
     <t>[MW]</t>
   </si>
@@ -384,9 +481,6 @@
     <t>Year where it is decommissioned (31.12.xxxx)</t>
   </si>
   <si>
-    <t>v0.0.3</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -400,6 +494,12 @@
   </si>
   <si>
     <t>Node_4</t>
+  </si>
+  <si>
+    <t>[°]</t>
+  </si>
+  <si>
+    <t>v0.0.3r</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1161,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1380,8 +1480,12 @@
       <c r="Q7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
+      <c r="R7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="T7" s="10" t="s">
         <v>51</v>
       </c>
@@ -1454,7 +1558,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="12" t="s">
@@ -1518,7 +1622,7 @@
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
       <c r="C10" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>5</v>
@@ -1578,7 +1682,7 @@
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>5</v>
@@ -1638,13 +1742,13 @@
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
       <c r="C12" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F12" s="25">
         <v>18</v>
@@ -1654,6 +1758,763 @@
       </c>
       <c r="H12" s="27">
         <v>0</v>
+      </c>
+      <c r="I12" s="26">
+        <v>150</v>
+      </c>
+      <c r="J12" s="28">
+        <v>87516.227433000007</v>
+      </c>
+      <c r="K12" s="28">
+        <v>0</v>
+      </c>
+      <c r="L12" s="30">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26">
+        <v>0</v>
+      </c>
+      <c r="P12" s="26">
+        <v>2010</v>
+      </c>
+      <c r="Q12" s="26">
+        <v>2030</v>
+      </c>
+      <c r="R12" s="24">
+        <v>47.990338000000001</v>
+      </c>
+      <c r="S12" s="24">
+        <v>16.378105000000001</v>
+      </c>
+      <c r="T12" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="U12" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="V12" s="3"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K16" s="2"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+    </row>
+    <row r="18" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+    </row>
+    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+    </row>
+    <row r="22" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+    </row>
+    <row r="23" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+    </row>
+    <row r="24" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+    </row>
+    <row r="25" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+    </row>
+    <row r="26" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFD5E5F-AB59-4FBF-B026-A717EE6BB3EE}">
+  <sheetPr>
+    <tabColor rgb="FF008080"/>
+  </sheetPr>
+  <dimension ref="A1:X27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="13.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="3" customWidth="1"/>
+    <col min="12" max="15" width="13.42578125" style="2" customWidth="1"/>
+    <col min="16" max="17" width="17.5703125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="P6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="T6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="U6" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="25">
+        <v>0</v>
+      </c>
+      <c r="G8" s="26">
+        <v>100</v>
+      </c>
+      <c r="H8" s="27">
+        <v>1</v>
+      </c>
+      <c r="I8" s="26">
+        <v>290</v>
+      </c>
+      <c r="J8" s="28">
+        <v>72641.801500000001</v>
+      </c>
+      <c r="K8" s="28">
+        <v>2</v>
+      </c>
+      <c r="L8" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26">
+        <v>0</v>
+      </c>
+      <c r="P8" s="26">
+        <v>2010</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>2030</v>
+      </c>
+      <c r="R8" s="24">
+        <v>47.491300000000003</v>
+      </c>
+      <c r="S8" s="24">
+        <v>12.818199999999999</v>
+      </c>
+      <c r="T8" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="U8" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="25">
+        <v>0</v>
+      </c>
+      <c r="G9" s="26">
+        <v>100</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1</v>
+      </c>
+      <c r="I9" s="26">
+        <v>290</v>
+      </c>
+      <c r="J9" s="28">
+        <v>80000</v>
+      </c>
+      <c r="K9" s="28">
+        <v>5</v>
+      </c>
+      <c r="L9" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26">
+        <v>2</v>
+      </c>
+      <c r="P9" s="26">
+        <v>2010</v>
+      </c>
+      <c r="Q9" s="26">
+        <v>2030</v>
+      </c>
+      <c r="R9" s="24">
+        <v>46.77</v>
+      </c>
+      <c r="S9" s="24">
+        <v>13.746700000000001</v>
+      </c>
+      <c r="T9" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="U9" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="V9" s="3"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="25">
+        <v>0</v>
+      </c>
+      <c r="G10" s="26">
+        <v>100</v>
+      </c>
+      <c r="H10" s="27">
+        <v>1</v>
+      </c>
+      <c r="I10" s="26">
+        <v>300</v>
+      </c>
+      <c r="J10" s="28">
+        <v>84467.2111</v>
+      </c>
+      <c r="K10" s="28">
+        <v>0</v>
+      </c>
+      <c r="L10" s="30">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26">
+        <v>0</v>
+      </c>
+      <c r="P10" s="26">
+        <v>2010</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>2030</v>
+      </c>
+      <c r="R10" s="24">
+        <v>48.239980000000003</v>
+      </c>
+      <c r="S10" s="24">
+        <v>16.538879999999999</v>
+      </c>
+      <c r="T10" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="U10" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="V10" s="3"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="25">
+        <v>0</v>
+      </c>
+      <c r="G11" s="26">
+        <v>100</v>
+      </c>
+      <c r="H11" s="27">
+        <v>1</v>
+      </c>
+      <c r="I11" s="26">
+        <v>300</v>
+      </c>
+      <c r="J11" s="28">
+        <v>84967.2111</v>
+      </c>
+      <c r="K11" s="28">
+        <v>0</v>
+      </c>
+      <c r="L11" s="30">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26">
+        <v>0</v>
+      </c>
+      <c r="P11" s="26">
+        <v>2010</v>
+      </c>
+      <c r="Q11" s="26">
+        <v>2030</v>
+      </c>
+      <c r="R11" s="24">
+        <v>48.345640000000003</v>
+      </c>
+      <c r="S11" s="24">
+        <v>16.667997</v>
+      </c>
+      <c r="T11" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="U11" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="V11" s="3"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0</v>
+      </c>
+      <c r="G12" s="26">
+        <v>100</v>
+      </c>
+      <c r="H12" s="27">
+        <v>1</v>
       </c>
       <c r="I12" s="26">
         <v>150</v>
@@ -1772,6 +2633,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1917,12 +2784,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1933,6 +2794,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1950,22 +2827,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update Power_VRES to v0.0.4r
Excl. to excl
long to lon
Corrections in human-readable column names
</commit_message>
<xml_diff>
--- a/examples/Power_VRES.xlsx
+++ b/examples/Power_VRES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C759EA27-F488-4721-B191-54D4E9491B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A4E800-E041-4883-9C14-F2584BA3D6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41895" yWindow="-19440" windowWidth="21600" windowHeight="12645" tabRatio="744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="107" r:id="rId1"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="85">
   <si>
     <t>[MW]</t>
   </si>
@@ -337,9 +337,6 @@
     <t>lat</t>
   </si>
   <si>
-    <t>long</t>
-  </si>
-  <si>
     <t>Excl.</t>
   </si>
   <si>
@@ -499,7 +496,19 @@
     <t>[°]</t>
   </si>
   <si>
-    <t>v0.0.3r</t>
+    <t>v0.0.4r</t>
+  </si>
+  <si>
+    <t>excl</t>
+  </si>
+  <si>
+    <t>Commision Year</t>
+  </si>
+  <si>
+    <t>Decommision Year</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
@@ -1158,12 +1167,12 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="F2"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1176,19 +1185,19 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>10</v>
@@ -1221,39 +1230,39 @@
         <v>12</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="T3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="U3" s="16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>10</v>
@@ -1295,154 +1304,154 @@
         <v>26</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="T4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="K5" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="M5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="N5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="O5" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="P5" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="P5" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="T5" s="19" t="s">
-        <v>69</v>
-      </c>
       <c r="U5" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>11</v>
@@ -1463,7 +1472,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M7" s="10" t="s">
         <v>16</v>
@@ -1475,22 +1484,22 @@
         <v>13</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
@@ -1547,10 +1556,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="T8" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U8" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
@@ -1558,7 +1567,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="12" t="s">
@@ -1609,10 +1618,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="T9" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U9" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U9" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V9" s="3"/>
       <c r="W9" s="13"/>
@@ -1622,7 +1631,7 @@
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
       <c r="C10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>5</v>
@@ -1669,10 +1678,10 @@
         <v>16.538879999999999</v>
       </c>
       <c r="T10" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U10" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V10" s="3"/>
       <c r="W10" s="13"/>
@@ -1682,7 +1691,7 @@
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>5</v>
@@ -1729,10 +1738,10 @@
         <v>16.667997</v>
       </c>
       <c r="T11" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U11" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U11" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V11" s="3"/>
       <c r="W11" s="13"/>
@@ -1742,13 +1751,13 @@
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
       <c r="C12" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="25">
         <v>18</v>
@@ -1789,10 +1798,10 @@
         <v>16.378105000000001</v>
       </c>
       <c r="T12" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U12" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U12" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V12" s="3"/>
       <c r="W12" s="13"/>
@@ -1884,8 +1893,9 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -1915,12 +1925,12 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="F2"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1933,19 +1943,19 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>10</v>
@@ -1978,39 +1988,39 @@
         <v>12</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="T3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="U3" s="16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>10</v>
@@ -2052,154 +2062,154 @@
         <v>26</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="T4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="K5" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="M5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="N5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="O5" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="P5" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="P5" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="T5" s="19" t="s">
-        <v>69</v>
-      </c>
       <c r="U5" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S6" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U6" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>11</v>
@@ -2220,7 +2230,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M7" s="10" t="s">
         <v>16</v>
@@ -2232,22 +2242,22 @@
         <v>13</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
@@ -2304,10 +2314,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="T8" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U8" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
@@ -2315,7 +2325,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="12" t="s">
@@ -2366,10 +2376,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="T9" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U9" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U9" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V9" s="3"/>
       <c r="W9" s="13"/>
@@ -2379,7 +2389,7 @@
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
       <c r="C10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>5</v>
@@ -2426,10 +2436,10 @@
         <v>16.538879999999999</v>
       </c>
       <c r="T10" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U10" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V10" s="3"/>
       <c r="W10" s="13"/>
@@ -2439,7 +2449,7 @@
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>5</v>
@@ -2486,10 +2496,10 @@
         <v>16.667997</v>
       </c>
       <c r="T11" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U11" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U11" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V11" s="3"/>
       <c r="W11" s="13"/>
@@ -2499,13 +2509,13 @@
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
       <c r="C12" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="25">
         <v>0</v>
@@ -2546,10 +2556,10 @@
         <v>16.378105000000001</v>
       </c>
       <c r="T12" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U12" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="U12" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="V12" s="3"/>
       <c r="W12" s="13"/>

</xml_diff>